<commit_message>
Arreglo cosas del ejecutable
</commit_message>
<xml_diff>
--- a/Archivos_necesarios/Maestro.xlsx
+++ b/Archivos_necesarios/Maestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rorro\Downloads\Trabajos Rodri\Vcard-generator\Archivos_necesarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67D4FF-5E34-408D-A7BE-62DA6A5F277E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14481A3-C31D-4319-8D79-0901917857B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9E361097-975F-41C7-87D4-E5BC70F11255}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Telefono</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Codigo</t>
+  </si>
+  <si>
+    <t>ALMACENES</t>
+  </si>
+  <si>
+    <t>CLIENTE B1</t>
+  </si>
+  <si>
+    <t>00000015</t>
+  </si>
+  <si>
+    <t>- - -3654789</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B85F34-FE2C-47A9-97DA-5A60EC7CE4C8}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,6 +443,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>